<commit_message>
running test at home 12
</commit_message>
<xml_diff>
--- a/login_class_26.xlsx
+++ b/login_class_26.xlsx
@@ -29,6 +29,22 @@
     </font>
     <font>
       <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="13"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
       <charset val="0"/>
       <color rgb="FFFF0000"/>
       <sz val="11"/>
@@ -37,7 +53,69 @@
     <font>
       <name val="Calibri"/>
       <charset val="0"/>
+      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <color theme="0"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FF3F3F3F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF9C0006"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -52,23 +130,20 @@
     <font>
       <name val="Calibri"/>
       <charset val="0"/>
-      <i val="1"/>
-      <color rgb="FF7F7F7F"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <b val="1"/>
+      <color rgb="FF9C6500"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <color rgb="FF006100"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <color rgb="FFFA7D00"/>
       <sz val="11"/>
       <scheme val="minor"/>
@@ -77,89 +152,6 @@
       <name val="Calibri"/>
       <charset val="0"/>
       <color rgb="FF3F3F76"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color rgb="FF3F3F3F"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FF0000FF"/>
-      <sz val="11"/>
-      <u val="single"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FF006100"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color rgb="FFFFFFFF"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="13"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FF9C0006"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FF9C6500"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FF800080"/>
-      <sz val="11"/>
-      <u val="single"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FFFA7D00"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -171,8 +163,16 @@
       <sz val="15"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <i val="1"/>
+      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill/>
     </fill>
@@ -193,187 +193,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -381,6 +381,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="00FFC7CE"/>
         <bgColor rgb="00FFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CCFFE5"/>
+        <bgColor rgb="00CCFFE5"/>
       </patternFill>
     </fill>
   </fills>
@@ -412,7 +418,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -428,21 +434,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -492,7 +483,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -505,157 +496,172 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="10" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="24" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="31" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="16" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="14" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="25" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="19" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="26" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="34" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="32" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="9" fillId="0" fontId="18" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="21" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="23" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="22" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="18" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="17" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="33" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="29" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="30" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="28" fontId="16" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="12" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="27" fontId="15" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="11" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="6" fillId="0" fontId="12" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="5" fillId="6" fontId="9" numFmtId="0">
+    <xf applyAlignment="1" borderId="0" fillId="30" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="8" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="14" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="32" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="25" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="11" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="5" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="9" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="4" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="33" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="8" fillId="0" fontId="16" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="15" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="29" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="23" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="26" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="24" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="17" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="21" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="34" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="28" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="19" fontId="14" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="18" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="16" fontId="12" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="13" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="0" fontId="10" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="4" fillId="7" fontId="9" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="44">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="9" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="4" fillId="8" fontId="0" numFmtId="0">
+    <xf applyAlignment="1" borderId="0" fillId="10" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="9" fillId="27" fontId="0" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="3" fillId="22" fontId="17" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="8" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="3" fillId="7" fontId="7" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="5" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="3" fillId="6" fontId="6" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="13" fontId="11" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="5" numFmtId="0">
+    <xf applyAlignment="1" borderId="0" fillId="20" fontId="15" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="7" fillId="0" fontId="8" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="19" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="18" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="6" fontId="5" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="13" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="42">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="1" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="165">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="6" fillId="12" fontId="11" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="31" fontId="6" numFmtId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="9">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="8" fillId="0" fontId="19" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="15" fontId="8" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="42">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="17" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="8" fillId="0" fontId="14" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="165">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="7" fillId="20" fontId="13" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="5" fontId="2" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="10" numFmtId="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -670,6 +676,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="1" fillId="35" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="36" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -992,7 +1001,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.800000000000001" defaultRowHeight="14.25" outlineLevelRow="4"/>
@@ -1031,9 +1040,9 @@
           <t>tutorial</t>
         </is>
       </c>
-      <c r="C2" s="4" t="inlineStr">
-        <is>
-          <t>PASS</t>
+      <c r="C2" s="5" t="inlineStr">
+        <is>
+          <t>FAIL</t>
         </is>
       </c>
     </row>
@@ -1048,7 +1057,7 @@
           <t>tutorial</t>
         </is>
       </c>
-      <c r="C3" s="2" t="inlineStr">
+      <c r="C3" s="5" t="inlineStr">
         <is>
           <t>FAIL</t>
         </is>
@@ -1065,7 +1074,7 @@
           <t>asdass</t>
         </is>
       </c>
-      <c r="C4" s="5" t="inlineStr">
+      <c r="C4" s="2" t="inlineStr">
         <is>
           <t>FAIL</t>
         </is>

</xml_diff>

<commit_message>
running test at home 13
</commit_message>
<xml_diff>
--- a/login_class_26.xlsx
+++ b/login_class_26.xlsx
@@ -1040,9 +1040,9 @@
           <t>tutorial</t>
         </is>
       </c>
-      <c r="C2" s="5" t="inlineStr">
-        <is>
-          <t>FAIL</t>
+      <c r="C2" s="6" t="inlineStr">
+        <is>
+          <t>PASS</t>
         </is>
       </c>
     </row>
@@ -1057,9 +1057,9 @@
           <t>tutorial</t>
         </is>
       </c>
-      <c r="C3" s="6" t="inlineStr">
-        <is>
-          <t>PASS</t>
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t>FAIL</t>
         </is>
       </c>
     </row>

</xml_diff>